<commit_message>
Avance en el programa 2
</commit_message>
<xml_diff>
--- a/Programa1/Resultado.xlsx
+++ b/Programa1/Resultado.xlsx
@@ -88,37 +88,37 @@
     <t>Mas Victorias:</t>
   </si>
   <si>
-    <t xml:space="preserve"> Barcelona</t>
+    <t xml:space="preserve"> / Barcelona</t>
   </si>
   <si>
     <t>Mas Empates:</t>
   </si>
   <si>
-    <t xml:space="preserve"> Real Sociedad</t>
+    <t xml:space="preserve"> / Real Sociedad</t>
   </si>
   <si>
     <t>Mas Derrotas:</t>
   </si>
   <si>
-    <t xml:space="preserve"> Rayo Vallecano</t>
+    <t xml:space="preserve"> / Rayo Vallecano</t>
   </si>
   <si>
     <t>Mas GF:</t>
   </si>
   <si>
-    <t xml:space="preserve"> Real Madrid</t>
+    <t xml:space="preserve"> / Real Madrid</t>
   </si>
   <si>
     <t>Menos GE:</t>
   </si>
   <si>
-    <t xml:space="preserve"> Atlético Madrid</t>
+    <t xml:space="preserve"> / Atlético Madrid</t>
   </si>
   <si>
     <t>Mas Puntos:</t>
   </si>
   <si>
-    <t xml:space="preserve"> Barcelona Real Madrid</t>
+    <t xml:space="preserve"> / Barcelona / Real Madrid</t>
   </si>
   <si>
     <t>Mas dif Puntos:</t>

</xml_diff>

<commit_message>
Punto 7 Programa 1
</commit_message>
<xml_diff>
--- a/Programa1/Resultado.xlsx
+++ b/Programa1/Resultado.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>Equipos</t>
   </si>
@@ -37,7 +37,7 @@
     <t>PTS</t>
   </si>
   <si>
-    <t>Pregunta7</t>
+    <t>Mayor dif. PTS</t>
   </si>
   <si>
     <t>Athletic Bilbao</t>
@@ -88,40 +88,67 @@
     <t>Mas Victorias:</t>
   </si>
   <si>
-    <t xml:space="preserve"> / Barcelona</t>
+    <t xml:space="preserve"> - Barcelona</t>
   </si>
   <si>
     <t>Mas Empates:</t>
   </si>
   <si>
-    <t xml:space="preserve"> / Real Sociedad</t>
+    <t xml:space="preserve"> - Real Sociedad</t>
   </si>
   <si>
     <t>Mas Derrotas:</t>
   </si>
   <si>
-    <t xml:space="preserve"> / Rayo Vallecano</t>
+    <t xml:space="preserve"> - Rayo Vallecano</t>
   </si>
   <si>
     <t>Mas GF:</t>
   </si>
   <si>
-    <t xml:space="preserve"> / Real Madrid</t>
+    <t xml:space="preserve"> - Real Madrid</t>
   </si>
   <si>
     <t>Menos GE:</t>
   </si>
   <si>
-    <t xml:space="preserve"> / Atlético Madrid</t>
+    <t xml:space="preserve"> - Atlético Madrid</t>
   </si>
   <si>
     <t>Mas Puntos:</t>
   </si>
   <si>
-    <t xml:space="preserve"> / Barcelona / Real Madrid</t>
+    <t xml:space="preserve"> - Barcelona - Real Madrid</t>
   </si>
   <si>
     <t>Mas dif Puntos:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Valencia</t>
+  </si>
+  <si>
+    <t>Mayor diferencia en temporada</t>
+  </si>
+  <si>
+    <t>Equipo</t>
+  </si>
+  <si>
+    <t>Dif</t>
+  </si>
+  <si>
+    <t>Temporada</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2012 - 2013 a 2013 - 2014/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2011 - 2012 a 2012 - 2013/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2013 - 2014 a 2014 - 2015/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2014 - 2015 a 2015 - 2016/ </t>
   </si>
 </sst>
 </file>
@@ -458,7 +485,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,7 +542,7 @@
         <v>281</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -541,7 +568,7 @@
         <v>388</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -567,7 +594,7 @@
         <v>463</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -593,7 +620,7 @@
         <v>224</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -619,7 +646,7 @@
         <v>209</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -645,7 +672,7 @@
         <v>199</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -671,7 +698,7 @@
         <v>218</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -697,7 +724,7 @@
         <v>258</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -723,7 +750,7 @@
         <v>226</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -749,7 +776,7 @@
         <v>463</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -775,7 +802,7 @@
         <v>266</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -801,7 +828,7 @@
         <v>291</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -827,7 +854,7 @@
         <v>296</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -917,10 +944,177 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C23" t="n">
-        <v>56</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s"/>
+      <c r="B24" t="s"/>
+      <c r="C24" t="s"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="n">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" t="n">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="n">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="n">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="n">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" t="n">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="n">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="n">
+        <v>12</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" t="n">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" t="n">
+        <v>15</v>
+      </c>
+      <c r="C36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" t="n">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" t="n">
+        <v>24</v>
+      </c>
+      <c r="C38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" t="n">
+        <v>33</v>
+      </c>
+      <c r="C39" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>